<commit_message>
a captcha file created for human verification
</commit_message>
<xml_diff>
--- a/Web Dev 2 Project Tracking_Rubric.xlsx
+++ b/Web Dev 2 Project Tracking_Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\wd2\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FDB348-7A5F-494F-9867-837311C0CCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A9668E-27E0-4794-98D9-E2714985B8AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1453,8 +1453,8 @@
   <dimension ref="A1:AC1155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B56" sqref="B56:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1471,7 @@
     <row r="1" spans="1:29" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; G203 &amp; " / Verified: " &amp; (H203 ) &amp; " / Verified with Deductions: " &amp; I203 &amp; " / Verified with Deductions &amp; Milestones: " &amp; J203</f>
-        <v>Unverified Marks: 2 / Verified: 34 / Verified with Deductions: 21 / Verified with Deductions &amp; Milestones: 21</v>
+        <v>Unverified Marks: 7 / Verified: 34 / Verified with Deductions: 21 / Verified with Deductions &amp; Milestones: 21</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -3382,7 +3382,7 @@
       </c>
       <c r="C50" s="11"/>
       <c r="D50" s="15" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11">
@@ -3390,7 +3390,7 @@
       </c>
       <c r="G50" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H50" s="3">
         <f>IF(D50 = "yes",F50, 0 )</f>
@@ -3427,7 +3427,7 @@
         <v>70</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="D51" s="11"/>
       <c r="E51" s="11"/>
@@ -3465,7 +3465,7 @@
         <v>71</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="D52" s="11"/>
       <c r="E52" s="11"/>
@@ -3503,7 +3503,7 @@
         <v>72</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="D53" s="11"/>
       <c r="E53" s="11"/>
@@ -3541,7 +3541,7 @@
         <v>73</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="D54" s="11"/>
       <c r="E54" s="11"/>
@@ -3579,7 +3579,7 @@
         <v>74</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>14</v>
+        <v>225</v>
       </c>
       <c r="D55" s="11"/>
       <c r="E55" s="11"/>
@@ -9405,7 +9405,7 @@
       <c r="F203" s="11"/>
       <c r="G203" s="3">
         <f t="shared" ref="G203:I203" si="2">SUM(G7:G202)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H203" s="3">
         <f t="shared" si="2"/>

</xml_diff>